<commit_message>
Excel templates reader implemented (except for loops)
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/output/out_basicXlsxTemplateResult.xlsx
+++ b/src/test/resources/xlsx/output/out_basicXlsxTemplateResult.xlsx
@@ -499,7 +499,6 @@
           <t>Jebt supports single properties.</t>
         </is>
       </c>
-      <c r="B1"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -507,7 +506,6 @@
           <t>Hello World!</t>
         </is>
       </c>
-      <c r="B2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -515,7 +513,6 @@
           <t>Even with Text formatting: Some bold World! But only the cell font will be preserved. Any text-section specific formatting will be discarded.</t>
         </is>
       </c>
-      <c r="B3"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -523,7 +520,6 @@
           <t>Sbet supports property chain, indexed properties, and mapped properties.</t>
         </is>
       </c>
-      <c r="B4"/>
     </row>
     <row r="5">
       <c r="A5"/>
@@ -532,7 +528,6 @@
           <t>The postal code of the third customer is 200093.</t>
         </is>
       </c>
-      <c r="C5"/>
     </row>
     <row r="6">
 </row>
@@ -542,7 +537,6 @@
           <t>Empty lines are not a problem.</t>
         </is>
       </c>
-      <c r="B7"/>
     </row>
     <row r="8">
 </row>
@@ -557,7 +551,6 @@
           <t>World folks, Let Jebt take on the World</t>
         </is>
       </c>
-      <c r="G9"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>